<commit_message>
Cleaning code for v.0.1 part I.
</commit_message>
<xml_diff>
--- a/data/observer_ids.xlsx
+++ b/data/observer_ids.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>HM</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>observer_coldef_type</t>
+  </si>
+  <si>
+    <t>RP</t>
+  </si>
+  <si>
+    <t>BO</t>
   </si>
 </sst>
 </file>
@@ -446,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.83203125" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0"/>
@@ -722,6 +728,28 @@
       </c>
       <c r="C24" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="23.25" customHeight="1">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="23.25" customHeight="1">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>